<commit_message>
Finalización de Hito 1
</commit_message>
<xml_diff>
--- a/Lineas Bases/SPVL/Linea Base 01/SPVL-CP.xlsx
+++ b/Lineas Bases/SPVL/Linea Base 01/SPVL-CP.xlsx
@@ -27,43 +27,43 @@
     <t>Rol</t>
   </si>
   <si>
-    <t>Jhoan Joseph Figueroa</t>
+    <t xml:space="preserve">Figueroa Garay, Jhoan Joseph </t>
   </si>
   <si>
     <t>Analista</t>
   </si>
   <si>
-    <t>Sebastian Ortiz Urbai</t>
+    <t xml:space="preserve">Ortiz Urbai, Sebastian </t>
   </si>
   <si>
     <t>Líder de proyecto y Desarrollador Full-Stack</t>
   </si>
   <si>
-    <t>Tejeda Echeagary Yosmar Aldair</t>
+    <t>Tejeda Echeagary, Yosmar Aldair</t>
   </si>
   <si>
     <t>Desarrollador back-end</t>
   </si>
   <si>
-    <t>Richard Saul Alvarez Huarsaya</t>
-  </si>
-  <si>
-    <t>Gerson Eduardo Aznaran Cabrera</t>
-  </si>
-  <si>
-    <t>Gustavo Alonso Tuyo Acero</t>
+    <t xml:space="preserve">Alvarez Huarsaya, Richard Saul </t>
+  </si>
+  <si>
+    <t>Aznaran Cabrera, Gerson Eduardo</t>
+  </si>
+  <si>
+    <t>Tuyo Acero, Gustavo Alonso</t>
   </si>
   <si>
     <t>Arquitecto de Software</t>
   </si>
   <si>
-    <t>Gerardo Ruben Paz Anchayhua</t>
+    <t>Paz Anchayhua, Gerardo Ruben</t>
   </si>
   <si>
     <t>Desarrollo Full-Stack</t>
   </si>
   <si>
-    <t>Chavez Campos Jean Pier</t>
+    <t>Chavez Campos,  Jean Pier</t>
   </si>
   <si>
     <t>Ruta del repositorio Github:  https://github.com/TestBox44/GCS-eLiquor.git</t>
@@ -177,26 +177,7 @@
     <t>Desarrollar del Plan de Proyecto</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Helvetica Neue"/>
-        <b/>
-        <i/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">Plan de Proyecto </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Helvetica Neue"/>
-        <b/>
-        <i/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>(PROJECT CHARTER)</t>
-    </r>
+    <t>Plan de Proyecto (PROJECT CHARTER)</t>
   </si>
   <si>
     <t>SPVL-PC.docx</t>
@@ -251,7 +232,7 @@
     <t>Documento de Especificación de historia de usuario HU-01</t>
   </si>
   <si>
-    <t>SPVL-DEHU-01.docx</t>
+    <t>HU_01_SPVL.docx</t>
   </si>
   <si>
     <t>Especificar Requisitos de HU-02</t>
@@ -260,7 +241,7 @@
     <t>Documento de Especificación de historia de usuario HU-02</t>
   </si>
   <si>
-    <t>SPVL-DEHU-02.docx</t>
+    <t>HU_02_SPVL.docx</t>
   </si>
   <si>
     <t>Especificar Requisitos de HU-03</t>
@@ -269,7 +250,7 @@
     <t>Documento de Especificación de historia de usuario HU-03</t>
   </si>
   <si>
-    <t>SPVL-DEHU-03.docx</t>
+    <t>HU_03_SPVL.docx</t>
   </si>
   <si>
     <t>Especificar Requisitos de HU-04</t>
@@ -278,7 +259,7 @@
     <t>Documento de Especificación de historia de usuario HU-04</t>
   </si>
   <si>
-    <t>SPVL-DEHU-04.docx</t>
+    <t>HU_04_SPVL.docx</t>
   </si>
   <si>
     <t>Especificar Requisitos de HU-05</t>
@@ -287,7 +268,7 @@
     <t>Documento de Especificación de historia de usuario HU-05</t>
   </si>
   <si>
-    <t>SPVL-DEHU-05.docx</t>
+    <t>HU_05_SPVL.docx</t>
   </si>
   <si>
     <t>Especificar Requisitos de HU-06</t>
@@ -296,7 +277,7 @@
     <t>Documento de Especificación de historia de usuario HU-06</t>
   </si>
   <si>
-    <t>SPVL-DEHU-06.docx</t>
+    <t>HU_06_SPVL.docx</t>
   </si>
   <si>
     <t>Especificar Requisitos de HU-07</t>
@@ -305,7 +286,7 @@
     <t>Documento de Especificación de historia de usuario HU-07</t>
   </si>
   <si>
-    <t>SPVL-DEHU-07.docx</t>
+    <t>HU_07_SPVL.docx</t>
   </si>
   <si>
     <t>Especificar Requisitos de HU-08</t>
@@ -314,7 +295,7 @@
     <t>Documento de Especificación de historia de usuario HU-08</t>
   </si>
   <si>
-    <t>SPVL-DEHU-08.docx</t>
+    <t>HU_08_SPVL.docx</t>
   </si>
   <si>
     <t>Proponer el diseño inicial de la Interface</t>
@@ -380,7 +361,7 @@
     <t>Reporte del Primer Sprint</t>
   </si>
   <si>
-    <t>SPVL-RPS.docx</t>
+    <t>REPORT_1SPRINT.docx</t>
   </si>
   <si>
     <t>Linea Base 1</t>
@@ -413,7 +394,7 @@
     <t>Reporte del Segundo Sprint</t>
   </si>
   <si>
-    <t>SPVL-RSP.docx</t>
+    <t>REPORT_2SPRINT.docx</t>
   </si>
   <si>
     <t>Linea Base 2</t>
@@ -485,7 +466,7 @@
     <t>Acta de cierre del proyecto</t>
   </si>
   <si>
-    <t>SPVL-ACP.docx</t>
+    <t>ACP-SPVL.docx</t>
   </si>
   <si>
     <t>Liena Base 3</t>
@@ -929,7 +910,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -938,7 +919,7 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -1012,7 +993,9 @@
     <xf borderId="17" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="4" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="17" fillId="6" fontId="13" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="17" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1317,7 +1300,7 @@
     <col customWidth="1" min="1" max="1" width="17.63"/>
     <col customWidth="1" min="2" max="2" width="68.25"/>
     <col customWidth="1" min="3" max="3" width="37.0"/>
-    <col customWidth="1" min="4" max="4" width="18.38"/>
+    <col customWidth="1" min="4" max="4" width="20.38"/>
     <col customWidth="1" min="5" max="5" width="70.38"/>
     <col customWidth="1" min="6" max="6" width="14.25"/>
     <col customWidth="1" min="7" max="7" width="13.88"/>
@@ -1696,7 +1679,7 @@
         <v>44832.0</v>
       </c>
       <c r="G40" s="41">
-        <v>44863.0</v>
+        <v>44833.0</v>
       </c>
       <c r="H40" s="45">
         <v>1.0</v>
@@ -1768,7 +1751,7 @@
         <v>44837.0</v>
       </c>
       <c r="H43" s="45">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -1791,7 +1774,7 @@
         <v>44837.0</v>
       </c>
       <c r="H44" s="45">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -1814,7 +1797,7 @@
         <v>44837.0</v>
       </c>
       <c r="H45" s="45">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -1837,7 +1820,7 @@
         <v>44837.0</v>
       </c>
       <c r="H46" s="45">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -1860,7 +1843,7 @@
         <v>44837.0</v>
       </c>
       <c r="H47" s="45">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -1883,7 +1866,7 @@
         <v>44837.0</v>
       </c>
       <c r="H48" s="45">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -1905,8 +1888,8 @@
       <c r="G49" s="41">
         <v>44838.0</v>
       </c>
-      <c r="H49" s="36">
-        <v>0.0</v>
+      <c r="H49" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
@@ -1916,7 +1899,7 @@
       <c r="C50" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="D50" s="38" t="s">
         <v>99</v>
       </c>
       <c r="E50" s="34" t="s">
@@ -1928,8 +1911,8 @@
       <c r="G50" s="41">
         <v>44838.0</v>
       </c>
-      <c r="H50" s="36">
-        <v>0.0</v>
+      <c r="H50" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -1951,8 +1934,8 @@
       <c r="G51" s="41">
         <v>44838.0</v>
       </c>
-      <c r="H51" s="36">
-        <v>0.0</v>
+      <c r="H51" s="45">
+        <v>1.0</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
@@ -1972,8 +1955,8 @@
       <c r="G52" s="53">
         <v>44840.0</v>
       </c>
-      <c r="H52" s="36">
-        <v>0.0</v>
+      <c r="H52" s="45">
+        <v>0.5</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -2004,7 +1987,7 @@
       <c r="C54" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="40" t="s">
+      <c r="D54" s="38" t="s">
         <v>110</v>
       </c>
       <c r="E54" s="34" t="s">
@@ -2027,7 +2010,7 @@
       <c r="C55" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D55" s="38" t="s">
         <v>114</v>
       </c>
       <c r="E55" s="34" t="s">
@@ -3544,8 +3527,11 @@
     <hyperlink r:id="rId11" ref="D47"/>
     <hyperlink r:id="rId12" ref="D48"/>
     <hyperlink r:id="rId13" ref="D49"/>
-    <hyperlink r:id="rId14" ref="D51"/>
+    <hyperlink r:id="rId14" ref="D50"/>
+    <hyperlink r:id="rId15" ref="D51"/>
+    <hyperlink r:id="rId16" ref="D54"/>
+    <hyperlink r:id="rId17" ref="D55"/>
   </hyperlinks>
-  <drawing r:id="rId15"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>